<commit_message>
REQ: updating excel data source - adding team-action, retrospective; deleting defect owner (defect assignee)
</commit_message>
<xml_diff>
--- a/agm-data-generator-1.01.xlsx
+++ b/agm-data-generator-1.01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="645" windowWidth="24675" windowHeight="12060" tabRatio="954" firstSheet="5" activeTab="21"/>
+    <workbookView xWindow="360" yWindow="645" windowWidth="24675" windowHeight="12060" tabRatio="954" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="18" r:id="rId1"/>
@@ -214,7 +214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7625" uniqueCount="1579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7633" uniqueCount="1579">
   <si>
     <t>SVN</t>
   </si>
@@ -4780,9 +4780,6 @@
     <t>https://gateway.saas.hp.com/msg/actions/showLogin</t>
   </si>
   <si>
-    <t>owner-username</t>
-  </si>
-  <si>
     <t>order</t>
   </si>
   <si>
@@ -4961,6 +4958,9 @@
   </si>
   <si>
     <t>The focus on the push was not clear</t>
+  </si>
+  <si>
+    <t>#owner-username</t>
   </si>
 </sst>
 </file>
@@ -5499,7 +5499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -5523,10 +5523,10 @@
         <v>29</v>
       </c>
       <c r="D1" s="32" t="s">
+        <v>1540</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>1541</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>1542</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5540,10 +5540,10 @@
         <v>322</v>
       </c>
       <c r="D2" s="32" t="s">
+        <v>1542</v>
+      </c>
+      <c r="E2" s="32" t="s">
         <v>1543</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>1544</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5551,10 +5551,10 @@
         <v>323</v>
       </c>
       <c r="D3" s="32" t="s">
+        <v>1544</v>
+      </c>
+      <c r="E3" s="32" t="s">
         <v>1545</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>1546</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -5562,10 +5562,10 @@
         <v>324</v>
       </c>
       <c r="D4" s="32" t="s">
+        <v>1546</v>
+      </c>
+      <c r="E4" s="32" t="s">
         <v>1547</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>1548</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5576,10 +5576,10 @@
         <v>322</v>
       </c>
       <c r="D5" s="32" t="s">
+        <v>1548</v>
+      </c>
+      <c r="E5" s="32" t="s">
         <v>1549</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>1550</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -5587,10 +5587,10 @@
         <v>323</v>
       </c>
       <c r="D6" s="32" t="s">
+        <v>1550</v>
+      </c>
+      <c r="E6" s="32" t="s">
         <v>1551</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>1552</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -5598,10 +5598,10 @@
         <v>324</v>
       </c>
       <c r="D7" s="32" t="s">
+        <v>1552</v>
+      </c>
+      <c r="E7" s="32" t="s">
         <v>1553</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>1554</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -5612,10 +5612,10 @@
         <v>322</v>
       </c>
       <c r="D8" s="32" t="s">
+        <v>1554</v>
+      </c>
+      <c r="E8" s="32" t="s">
         <v>1555</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>1556</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -5623,10 +5623,10 @@
         <v>323</v>
       </c>
       <c r="D9" s="32" t="s">
+        <v>1556</v>
+      </c>
+      <c r="E9" s="32" t="s">
         <v>1557</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>1558</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -5634,10 +5634,10 @@
         <v>324</v>
       </c>
       <c r="D10" s="32" t="s">
+        <v>1558</v>
+      </c>
+      <c r="E10" s="32" t="s">
         <v>1559</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>1560</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -5648,10 +5648,10 @@
         <v>322</v>
       </c>
       <c r="D11" s="32" t="s">
+        <v>1560</v>
+      </c>
+      <c r="E11" s="32" t="s">
         <v>1561</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>1562</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -5659,10 +5659,10 @@
         <v>323</v>
       </c>
       <c r="D12" s="32" t="s">
+        <v>1562</v>
+      </c>
+      <c r="E12" s="32" t="s">
         <v>1563</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>1564</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -5670,10 +5670,10 @@
         <v>324</v>
       </c>
       <c r="D13" s="32" t="s">
+        <v>1564</v>
+      </c>
+      <c r="E13" s="32" t="s">
         <v>1565</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>1566</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -5684,10 +5684,10 @@
         <v>322</v>
       </c>
       <c r="D14" s="32" t="s">
+        <v>1566</v>
+      </c>
+      <c r="E14" s="32" t="s">
         <v>1567</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>1568</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -5695,10 +5695,10 @@
         <v>323</v>
       </c>
       <c r="D15" s="32" t="s">
+        <v>1568</v>
+      </c>
+      <c r="E15" s="32" t="s">
         <v>1569</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>1570</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -5706,10 +5706,10 @@
         <v>324</v>
       </c>
       <c r="D16" s="32" t="s">
+        <v>1570</v>
+      </c>
+      <c r="E16" s="32" t="s">
         <v>1571</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>1572</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -5720,10 +5720,10 @@
         <v>322</v>
       </c>
       <c r="D17" s="32" t="s">
+        <v>1572</v>
+      </c>
+      <c r="E17" s="32" t="s">
         <v>1573</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>1574</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -5731,10 +5731,10 @@
         <v>323</v>
       </c>
       <c r="D18" s="32" t="s">
+        <v>1574</v>
+      </c>
+      <c r="E18" s="32" t="s">
         <v>1575</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>1576</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -5742,10 +5742,10 @@
         <v>324</v>
       </c>
       <c r="D19" s="32" t="s">
+        <v>1576</v>
+      </c>
+      <c r="E19" s="32" t="s">
         <v>1577</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>1578</v>
       </c>
     </row>
   </sheetData>
@@ -5755,22 +5755,22 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G149"/>
+  <dimension ref="A1:Q149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:E149"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="H1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="32" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="32"/>
-    <col min="3" max="3" width="96.85546875" style="32" customWidth="1"/>
+    <col min="3" max="3" width="89" style="32" customWidth="1"/>
     <col min="4" max="4" width="15" style="32" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" style="32" customWidth="1"/>
     <col min="6" max="6" width="7.5703125" style="32" customWidth="1"/>
     <col min="7" max="7" width="18.140625" style="32" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="32"/>
+    <col min="18" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -8322,10 +8322,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K241"/>
+  <dimension ref="A1:J241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B215" sqref="B215"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8333,17 +8333,16 @@
     <col min="1" max="1" width="9.140625" style="32"/>
     <col min="2" max="2" width="11.7109375" style="32" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" style="32" customWidth="1"/>
-    <col min="4" max="4" width="77.140625" style="32" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" style="32" customWidth="1"/>
+    <col min="4" max="4" width="23" style="32" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="32" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="32"/>
     <col min="8" max="8" width="18" style="32" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="32" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="32" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="32" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="32"/>
+    <col min="9" max="9" width="16.42578125" style="32" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="32" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>10</v>
       </c>
@@ -8369,16 +8368,13 @@
         <v>8</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>78</v>
+        <v>303</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>303</v>
-      </c>
-      <c r="K1" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>1706</v>
       </c>
@@ -8403,17 +8399,14 @@
       <c r="H2" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="I2" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="J2" s="32" t="s">
+      <c r="I2" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1707</v>
       </c>
@@ -8430,14 +8423,14 @@
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
-      <c r="J3" s="32" t="s">
+      <c r="I3" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="J3" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>1708</v>
       </c>
@@ -8454,14 +8447,14 @@
       </c>
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
-      <c r="J4" s="32" t="s">
+      <c r="I4" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="J4" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>1709</v>
       </c>
@@ -8475,14 +8468,14 @@
         <v>4</v>
       </c>
       <c r="G5" s="22"/>
-      <c r="J5" s="32" t="s">
+      <c r="I5" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K5" s="22" t="s">
+      <c r="J5" s="22" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>1710</v>
       </c>
@@ -8496,14 +8489,14 @@
         <v>13</v>
       </c>
       <c r="G6" s="22"/>
-      <c r="J6" s="32" t="s">
+      <c r="I6" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="J6" s="22" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>1711</v>
       </c>
@@ -8517,14 +8510,14 @@
         <v>13</v>
       </c>
       <c r="G7" s="22"/>
-      <c r="J7" s="32" t="s">
+      <c r="I7" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="J7" s="22" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>1712</v>
       </c>
@@ -8538,14 +8531,14 @@
         <v>302</v>
       </c>
       <c r="G8" s="22"/>
-      <c r="J8" s="32" t="s">
+      <c r="I8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="J8" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>1713</v>
       </c>
@@ -8559,14 +8552,14 @@
         <v>302</v>
       </c>
       <c r="G9" s="22"/>
-      <c r="J9" s="32" t="s">
+      <c r="I9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="22" t="s">
+      <c r="J9" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>1714</v>
       </c>
@@ -8580,14 +8573,14 @@
         <v>302</v>
       </c>
       <c r="G10" s="22"/>
-      <c r="J10" s="32" t="s">
+      <c r="I10" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="J10" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>1715</v>
       </c>
@@ -8601,14 +8594,14 @@
         <v>9</v>
       </c>
       <c r="G11" s="22"/>
-      <c r="J11" s="32" t="s">
+      <c r="I11" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="J11" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>1716</v>
       </c>
@@ -8622,14 +8615,14 @@
         <v>302</v>
       </c>
       <c r="G12" s="22"/>
-      <c r="J12" s="32" t="s">
+      <c r="I12" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="J12" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>1717</v>
       </c>
@@ -8643,14 +8636,14 @@
         <v>9</v>
       </c>
       <c r="G13" s="22"/>
-      <c r="J13" s="32" t="s">
+      <c r="I13" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K13" s="22" t="s">
+      <c r="J13" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>1718</v>
       </c>
@@ -8664,14 +8657,14 @@
         <v>302</v>
       </c>
       <c r="G14" s="22"/>
-      <c r="J14" s="32" t="s">
+      <c r="I14" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K14" s="22" t="s">
+      <c r="J14" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>1719</v>
       </c>
@@ -8685,14 +8678,14 @@
         <v>302</v>
       </c>
       <c r="G15" s="22"/>
-      <c r="J15" s="32" t="s">
+      <c r="I15" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="22" t="s">
+      <c r="J15" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>1720</v>
       </c>
@@ -8706,14 +8699,14 @@
         <v>9</v>
       </c>
       <c r="G16" s="22"/>
-      <c r="J16" s="32" t="s">
+      <c r="I16" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="J16" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>1721</v>
       </c>
@@ -8727,14 +8720,14 @@
         <v>302</v>
       </c>
       <c r="G17" s="22"/>
-      <c r="J17" s="32" t="s">
+      <c r="I17" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="22" t="s">
+      <c r="J17" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>1722</v>
       </c>
@@ -8748,14 +8741,14 @@
         <v>4</v>
       </c>
       <c r="G18" s="22"/>
-      <c r="J18" s="32" t="s">
+      <c r="I18" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K18" s="22" t="s">
+      <c r="J18" s="22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>1723</v>
       </c>
@@ -8769,14 +8762,14 @@
         <v>9</v>
       </c>
       <c r="G19" s="22"/>
-      <c r="J19" s="32" t="s">
+      <c r="I19" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K19" s="22" t="s">
+      <c r="J19" s="22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>1724</v>
       </c>
@@ -8790,14 +8783,14 @@
         <v>9</v>
       </c>
       <c r="G20" s="22"/>
-      <c r="J20" s="32" t="s">
+      <c r="I20" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K20" s="22" t="s">
+      <c r="J20" s="22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>1725</v>
       </c>
@@ -8811,14 +8804,14 @@
         <v>13</v>
       </c>
       <c r="G21" s="22"/>
-      <c r="J21" s="32" t="s">
+      <c r="I21" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K21" s="22" t="s">
+      <c r="J21" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>1726</v>
       </c>
@@ -8832,14 +8825,14 @@
         <v>9</v>
       </c>
       <c r="G22" s="22"/>
-      <c r="J22" s="32" t="s">
+      <c r="I22" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K22" s="22" t="s">
+      <c r="J22" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>1727</v>
       </c>
@@ -8853,14 +8846,14 @@
         <v>4</v>
       </c>
       <c r="G23" s="22"/>
-      <c r="J23" s="32" t="s">
+      <c r="I23" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K23" s="22" t="s">
+      <c r="J23" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>1728</v>
       </c>
@@ -8874,14 +8867,14 @@
         <v>302</v>
       </c>
       <c r="G24" s="22"/>
-      <c r="J24" s="32" t="s">
+      <c r="I24" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K24" s="22" t="s">
+      <c r="J24" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>1729</v>
       </c>
@@ -8895,14 +8888,14 @@
         <v>302</v>
       </c>
       <c r="G25" s="22"/>
-      <c r="J25" s="32" t="s">
+      <c r="I25" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K25" s="22" t="s">
+      <c r="J25" s="22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
         <v>1730</v>
       </c>
@@ -8916,14 +8909,14 @@
         <v>4</v>
       </c>
       <c r="G26" s="22"/>
-      <c r="J26" s="32" t="s">
+      <c r="I26" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K26" s="22" t="s">
+      <c r="J26" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>1731</v>
       </c>
@@ -8937,14 +8930,14 @@
         <v>9</v>
       </c>
       <c r="G27" s="22"/>
-      <c r="J27" s="32" t="s">
+      <c r="I27" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K27" s="22" t="s">
+      <c r="J27" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>1732</v>
       </c>
@@ -8958,14 +8951,14 @@
         <v>9</v>
       </c>
       <c r="G28" s="22"/>
-      <c r="J28" s="32" t="s">
+      <c r="I28" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K28" s="22" t="s">
+      <c r="J28" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>1733</v>
       </c>
@@ -8979,14 +8972,14 @@
         <v>9</v>
       </c>
       <c r="G29" s="22"/>
-      <c r="J29" s="32" t="s">
+      <c r="I29" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K29" s="22" t="s">
+      <c r="J29" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>1734</v>
       </c>
@@ -9000,14 +8993,14 @@
         <v>9</v>
       </c>
       <c r="G30" s="22"/>
-      <c r="J30" s="32" t="s">
+      <c r="I30" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K30" s="22" t="s">
+      <c r="J30" s="22" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>1735</v>
       </c>
@@ -9021,14 +9014,14 @@
         <v>4</v>
       </c>
       <c r="G31" s="22"/>
-      <c r="J31" s="32" t="s">
+      <c r="I31" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K31" s="22" t="s">
+      <c r="J31" s="22" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>1736</v>
       </c>
@@ -9042,14 +9035,14 @@
         <v>302</v>
       </c>
       <c r="G32" s="22"/>
-      <c r="J32" s="32" t="s">
+      <c r="I32" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K32" s="22" t="s">
+      <c r="J32" s="22" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>1737</v>
       </c>
@@ -9063,14 +9056,14 @@
         <v>302</v>
       </c>
       <c r="G33" s="22"/>
-      <c r="J33" s="32" t="s">
+      <c r="I33" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K33" s="22" t="s">
+      <c r="J33" s="22" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>1738</v>
       </c>
@@ -9084,14 +9077,14 @@
         <v>302</v>
       </c>
       <c r="G34" s="22"/>
-      <c r="J34" s="32" t="s">
+      <c r="I34" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K34" s="22" t="s">
+      <c r="J34" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>1739</v>
       </c>
@@ -9105,14 +9098,14 @@
         <v>13</v>
       </c>
       <c r="G35" s="22"/>
-      <c r="J35" s="32" t="s">
+      <c r="I35" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K35" s="22" t="s">
+      <c r="J35" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>1740</v>
       </c>
@@ -9126,14 +9119,14 @@
         <v>13</v>
       </c>
       <c r="G36" s="22"/>
-      <c r="J36" s="32" t="s">
+      <c r="I36" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K36" s="22" t="s">
+      <c r="J36" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>1741</v>
       </c>
@@ -9147,14 +9140,14 @@
         <v>9</v>
       </c>
       <c r="G37" s="22"/>
-      <c r="J37" s="32" t="s">
+      <c r="I37" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K37" s="22" t="s">
+      <c r="J37" s="22" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>1742</v>
       </c>
@@ -9168,14 +9161,14 @@
         <v>302</v>
       </c>
       <c r="G38" s="22"/>
-      <c r="J38" s="32" t="s">
+      <c r="I38" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K38" s="22" t="s">
+      <c r="J38" s="22" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>1743</v>
       </c>
@@ -9189,14 +9182,14 @@
         <v>13</v>
       </c>
       <c r="G39" s="22"/>
-      <c r="J39" s="32" t="s">
+      <c r="I39" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K39" s="22" t="s">
+      <c r="J39" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="14">
         <v>1744</v>
       </c>
@@ -9210,14 +9203,14 @@
         <v>302</v>
       </c>
       <c r="G40" s="22"/>
-      <c r="J40" s="32" t="s">
+      <c r="I40" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K40" s="22" t="s">
+      <c r="J40" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>1745</v>
       </c>
@@ -9231,14 +9224,14 @@
         <v>9</v>
       </c>
       <c r="G41" s="22"/>
-      <c r="J41" s="32" t="s">
+      <c r="I41" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K41" s="22" t="s">
+      <c r="J41" s="22" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
         <v>1746</v>
       </c>
@@ -9252,14 +9245,14 @@
         <v>13</v>
       </c>
       <c r="G42" s="22"/>
-      <c r="J42" s="32" t="s">
+      <c r="I42" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K42" s="22" t="s">
+      <c r="J42" s="22" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>1747</v>
       </c>
@@ -9273,14 +9266,14 @@
         <v>13</v>
       </c>
       <c r="G43" s="22"/>
-      <c r="J43" s="32" t="s">
+      <c r="I43" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K43" s="22" t="s">
+      <c r="J43" s="22" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="14">
         <v>1748</v>
       </c>
@@ -9294,14 +9287,14 @@
         <v>302</v>
       </c>
       <c r="G44" s="22"/>
-      <c r="J44" s="32" t="s">
+      <c r="I44" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K44" s="22" t="s">
+      <c r="J44" s="22" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>1749</v>
       </c>
@@ -9315,14 +9308,14 @@
         <v>302</v>
       </c>
       <c r="G45" s="22"/>
-      <c r="J45" s="32" t="s">
+      <c r="I45" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K45" s="22" t="s">
+      <c r="J45" s="22" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="14">
         <v>1750</v>
       </c>
@@ -9336,14 +9329,14 @@
         <v>9</v>
       </c>
       <c r="G46" s="22"/>
-      <c r="J46" s="32" t="s">
+      <c r="I46" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K46" s="22" t="s">
+      <c r="J46" s="22" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>1751</v>
       </c>
@@ -9357,14 +9350,14 @@
         <v>302</v>
       </c>
       <c r="G47" s="22"/>
-      <c r="J47" s="32" t="s">
+      <c r="I47" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="22" t="s">
+      <c r="J47" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
         <v>1752</v>
       </c>
@@ -9378,14 +9371,14 @@
         <v>302</v>
       </c>
       <c r="G48" s="22"/>
-      <c r="J48" s="32" t="s">
+      <c r="I48" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K48" s="22" t="s">
+      <c r="J48" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <v>1753</v>
       </c>
@@ -9399,14 +9392,14 @@
         <v>302</v>
       </c>
       <c r="G49" s="22"/>
-      <c r="J49" s="32" t="s">
+      <c r="I49" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K49" s="22" t="s">
+      <c r="J49" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="14">
         <v>1754</v>
       </c>
@@ -9420,14 +9413,14 @@
         <v>9</v>
       </c>
       <c r="G50" s="22"/>
-      <c r="J50" s="32" t="s">
+      <c r="I50" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K50" s="22" t="s">
+      <c r="J50" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <v>1755</v>
       </c>
@@ -9441,14 +9434,14 @@
         <v>302</v>
       </c>
       <c r="G51" s="22"/>
-      <c r="J51" s="32" t="s">
+      <c r="I51" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K51" s="22" t="s">
+      <c r="J51" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="14">
         <v>1756</v>
       </c>
@@ -9462,14 +9455,14 @@
         <v>9</v>
       </c>
       <c r="G52" s="22"/>
-      <c r="J52" s="32" t="s">
+      <c r="I52" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K52" s="22" t="s">
+      <c r="J52" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <v>1757</v>
       </c>
@@ -9483,14 +9476,14 @@
         <v>302</v>
       </c>
       <c r="G53" s="22"/>
-      <c r="J53" s="32" t="s">
+      <c r="I53" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K53" s="22" t="s">
+      <c r="J53" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="14">
         <v>1758</v>
       </c>
@@ -9504,14 +9497,14 @@
         <v>4</v>
       </c>
       <c r="G54" s="22"/>
-      <c r="J54" s="32" t="s">
+      <c r="I54" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K54" s="22" t="s">
+      <c r="J54" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <v>1759</v>
       </c>
@@ -9525,14 +9518,14 @@
         <v>302</v>
       </c>
       <c r="G55" s="22"/>
-      <c r="J55" s="32" t="s">
+      <c r="I55" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K55" s="22" t="s">
+      <c r="J55" s="22" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="14">
         <v>1760</v>
       </c>
@@ -9546,14 +9539,14 @@
         <v>302</v>
       </c>
       <c r="G56" s="22"/>
-      <c r="J56" s="32" t="s">
+      <c r="I56" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K56" s="22" t="s">
+      <c r="J56" s="22" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <v>1761</v>
       </c>
@@ -9567,14 +9560,14 @@
         <v>13</v>
       </c>
       <c r="G57" s="22"/>
-      <c r="J57" s="32" t="s">
+      <c r="I57" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K57" s="22" t="s">
+      <c r="J57" s="22" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="14">
         <v>1762</v>
       </c>
@@ -9588,14 +9581,14 @@
         <v>4</v>
       </c>
       <c r="G58" s="22"/>
-      <c r="J58" s="32" t="s">
+      <c r="I58" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K58" s="22" t="s">
+      <c r="J58" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <v>1763</v>
       </c>
@@ -9609,14 +9602,14 @@
         <v>9</v>
       </c>
       <c r="G59" s="22"/>
-      <c r="J59" s="32" t="s">
+      <c r="I59" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K59" s="22" t="s">
+      <c r="J59" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="14">
         <v>1764</v>
       </c>
@@ -9630,14 +9623,14 @@
         <v>302</v>
       </c>
       <c r="G60" s="22"/>
-      <c r="J60" s="32" t="s">
+      <c r="I60" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K60" s="22" t="s">
+      <c r="J60" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <v>1765</v>
       </c>
@@ -9651,14 +9644,14 @@
         <v>302</v>
       </c>
       <c r="G61" s="22"/>
-      <c r="J61" s="32" t="s">
+      <c r="I61" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K61" s="22" t="s">
+      <c r="J61" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="14">
         <v>1766</v>
       </c>
@@ -9672,14 +9665,14 @@
         <v>4</v>
       </c>
       <c r="G62" s="22"/>
-      <c r="J62" s="32" t="s">
+      <c r="I62" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K62" s="22" t="s">
+      <c r="J62" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <v>1767</v>
       </c>
@@ -9693,14 +9686,14 @@
         <v>302</v>
       </c>
       <c r="G63" s="22"/>
-      <c r="J63" s="32" t="s">
+      <c r="I63" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K63" s="22" t="s">
+      <c r="J63" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="14">
         <v>1768</v>
       </c>
@@ -9714,14 +9707,14 @@
         <v>302</v>
       </c>
       <c r="G64" s="22"/>
-      <c r="J64" s="32" t="s">
+      <c r="I64" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K64" s="22" t="s">
+      <c r="J64" s="22" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <v>1769</v>
       </c>
@@ -9735,14 +9728,14 @@
         <v>302</v>
       </c>
       <c r="G65" s="22"/>
-      <c r="J65" s="32" t="s">
+      <c r="I65" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K65" s="22" t="s">
+      <c r="J65" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="14">
         <v>1770</v>
       </c>
@@ -9756,14 +9749,14 @@
         <v>9</v>
       </c>
       <c r="G66" s="22"/>
-      <c r="J66" s="32" t="s">
+      <c r="I66" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K66" s="22" t="s">
+      <c r="J66" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <v>1771</v>
       </c>
@@ -9777,14 +9770,14 @@
         <v>9</v>
       </c>
       <c r="G67" s="22"/>
-      <c r="J67" s="32" t="s">
+      <c r="I67" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K67" s="22" t="s">
+      <c r="J67" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="14">
         <v>1772</v>
       </c>
@@ -9798,14 +9791,14 @@
         <v>302</v>
       </c>
       <c r="G68" s="22"/>
-      <c r="J68" s="32" t="s">
+      <c r="I68" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K68" s="22" t="s">
+      <c r="J68" s="22" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <v>1773</v>
       </c>
@@ -9819,14 +9812,14 @@
         <v>302</v>
       </c>
       <c r="G69" s="22"/>
-      <c r="J69" s="32" t="s">
+      <c r="I69" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K69" s="22" t="s">
+      <c r="J69" s="22" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="14">
         <v>1774</v>
       </c>
@@ -9840,14 +9833,14 @@
         <v>302</v>
       </c>
       <c r="G70" s="22"/>
-      <c r="J70" s="32" t="s">
+      <c r="I70" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K70" s="22" t="s">
+      <c r="J70" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <v>1775</v>
       </c>
@@ -9861,14 +9854,14 @@
         <v>13</v>
       </c>
       <c r="G71" s="22"/>
-      <c r="J71" s="32" t="s">
+      <c r="I71" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K71" s="22" t="s">
+      <c r="J71" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="14">
         <v>1776</v>
       </c>
@@ -9882,14 +9875,14 @@
         <v>13</v>
       </c>
       <c r="G72" s="22"/>
-      <c r="J72" s="32" t="s">
+      <c r="I72" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K72" s="22" t="s">
+      <c r="J72" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <v>1777</v>
       </c>
@@ -9903,14 +9896,14 @@
         <v>9</v>
       </c>
       <c r="G73" s="22"/>
-      <c r="J73" s="32" t="s">
+      <c r="I73" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K73" s="22" t="s">
+      <c r="J73" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="14">
         <v>1778</v>
       </c>
@@ -9924,14 +9917,14 @@
         <v>302</v>
       </c>
       <c r="G74" s="22"/>
-      <c r="J74" s="32" t="s">
+      <c r="I74" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K74" s="22" t="s">
+      <c r="J74" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <v>1779</v>
       </c>
@@ -9945,14 +9938,14 @@
         <v>13</v>
       </c>
       <c r="G75" s="22"/>
-      <c r="J75" s="32" t="s">
+      <c r="I75" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K75" s="22" t="s">
+      <c r="J75" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="14">
         <v>1780</v>
       </c>
@@ -9966,14 +9959,14 @@
         <v>302</v>
       </c>
       <c r="G76" s="22"/>
-      <c r="J76" s="32" t="s">
+      <c r="I76" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K76" s="22" t="s">
+      <c r="J76" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <v>1781</v>
       </c>
@@ -9987,14 +9980,14 @@
         <v>4</v>
       </c>
       <c r="G77" s="22"/>
-      <c r="J77" s="32" t="s">
+      <c r="I77" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K77" s="22" t="s">
+      <c r="J77" s="22" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="14">
         <v>1782</v>
       </c>
@@ -10008,14 +10001,14 @@
         <v>13</v>
       </c>
       <c r="G78" s="22"/>
-      <c r="J78" s="32" t="s">
+      <c r="I78" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K78" s="22" t="s">
+      <c r="J78" s="22" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <v>1783</v>
       </c>
@@ -10029,14 +10022,14 @@
         <v>13</v>
       </c>
       <c r="G79" s="22"/>
-      <c r="J79" s="32" t="s">
+      <c r="I79" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K79" s="22" t="s">
+      <c r="J79" s="22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="14">
         <v>1784</v>
       </c>
@@ -10050,14 +10043,14 @@
         <v>302</v>
       </c>
       <c r="G80" s="22"/>
-      <c r="J80" s="32" t="s">
+      <c r="I80" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K80" s="22" t="s">
+      <c r="J80" s="22" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <v>1785</v>
       </c>
@@ -10071,14 +10064,14 @@
         <v>302</v>
       </c>
       <c r="G81" s="22"/>
-      <c r="J81" s="32" t="s">
+      <c r="I81" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K81" s="22" t="s">
+      <c r="J81" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="14">
         <v>1786</v>
       </c>
@@ -10092,14 +10085,14 @@
         <v>302</v>
       </c>
       <c r="G82" s="22"/>
-      <c r="J82" s="32" t="s">
+      <c r="I82" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K82" s="22" t="s">
+      <c r="J82" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <v>1787</v>
       </c>
@@ -10113,14 +10106,14 @@
         <v>302</v>
       </c>
       <c r="G83" s="22"/>
-      <c r="J83" s="32" t="s">
+      <c r="I83" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K83" s="22" t="s">
+      <c r="J83" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="14">
         <v>1788</v>
       </c>
@@ -10134,14 +10127,14 @@
         <v>302</v>
       </c>
       <c r="G84" s="22"/>
-      <c r="J84" s="32" t="s">
+      <c r="I84" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K84" s="22" t="s">
+      <c r="J84" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <v>1789</v>
       </c>
@@ -10155,14 +10148,14 @@
         <v>9</v>
       </c>
       <c r="G85" s="22"/>
-      <c r="J85" s="32" t="s">
+      <c r="I85" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K85" s="22" t="s">
+      <c r="J85" s="22" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="14">
         <v>1790</v>
       </c>
@@ -10176,14 +10169,14 @@
         <v>9</v>
       </c>
       <c r="G86" s="22"/>
-      <c r="J86" s="32" t="s">
+      <c r="I86" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K86" s="22" t="s">
+      <c r="J86" s="22" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <v>1791</v>
       </c>
@@ -10197,14 +10190,14 @@
         <v>302</v>
       </c>
       <c r="G87" s="22"/>
-      <c r="J87" s="32" t="s">
+      <c r="I87" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K87" s="22" t="s">
+      <c r="J87" s="22" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="14">
         <v>1792</v>
       </c>
@@ -10218,14 +10211,14 @@
         <v>302</v>
       </c>
       <c r="G88" s="22"/>
-      <c r="J88" s="32" t="s">
+      <c r="I88" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K88" s="22" t="s">
+      <c r="J88" s="22" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <v>1793</v>
       </c>
@@ -10239,14 +10232,14 @@
         <v>302</v>
       </c>
       <c r="G89" s="22"/>
-      <c r="J89" s="32" t="s">
+      <c r="I89" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K89" s="22" t="s">
+      <c r="J89" s="22" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="14">
         <v>1794</v>
       </c>
@@ -10260,14 +10253,14 @@
         <v>4</v>
       </c>
       <c r="G90" s="22"/>
-      <c r="J90" s="32" t="s">
+      <c r="I90" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K90" s="22" t="s">
+      <c r="J90" s="22" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <v>1795</v>
       </c>
@@ -10281,14 +10274,14 @@
         <v>302</v>
       </c>
       <c r="G91" s="22"/>
-      <c r="J91" s="32" t="s">
+      <c r="I91" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K91" s="22" t="s">
+      <c r="J91" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="14">
         <v>1796</v>
       </c>
@@ -10302,14 +10295,14 @@
         <v>302</v>
       </c>
       <c r="G92" s="22"/>
-      <c r="J92" s="32" t="s">
+      <c r="I92" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K92" s="22" t="s">
+      <c r="J92" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <v>1797</v>
       </c>
@@ -10323,14 +10316,14 @@
         <v>13</v>
       </c>
       <c r="G93" s="22"/>
-      <c r="J93" s="32" t="s">
+      <c r="I93" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K93" s="22" t="s">
+      <c r="J93" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="14">
         <v>1798</v>
       </c>
@@ -10344,14 +10337,14 @@
         <v>4</v>
       </c>
       <c r="G94" s="22"/>
-      <c r="J94" s="32" t="s">
+      <c r="I94" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K94" s="22" t="s">
+      <c r="J94" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <v>1799</v>
       </c>
@@ -10365,14 +10358,14 @@
         <v>4</v>
       </c>
       <c r="G95" s="22"/>
-      <c r="J95" s="32" t="s">
+      <c r="I95" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K95" s="22" t="s">
+      <c r="J95" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="14">
         <v>1800</v>
       </c>
@@ -10386,14 +10379,14 @@
         <v>302</v>
       </c>
       <c r="G96" s="22"/>
-      <c r="J96" s="32" t="s">
+      <c r="I96" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K96" s="22" t="s">
+      <c r="J96" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <v>1801</v>
       </c>
@@ -10407,14 +10400,14 @@
         <v>9</v>
       </c>
       <c r="G97" s="22"/>
-      <c r="J97" s="32" t="s">
+      <c r="I97" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K97" s="22" t="s">
+      <c r="J97" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="14">
         <v>1802</v>
       </c>
@@ -10428,14 +10421,14 @@
         <v>9</v>
       </c>
       <c r="G98" s="22"/>
-      <c r="J98" s="32" t="s">
+      <c r="I98" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K98" s="22" t="s">
+      <c r="J98" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <v>1803</v>
       </c>
@@ -10449,14 +10442,14 @@
         <v>302</v>
       </c>
       <c r="G99" s="22"/>
-      <c r="J99" s="32" t="s">
+      <c r="I99" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K99" s="22" t="s">
+      <c r="J99" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="14">
         <v>1804</v>
       </c>
@@ -10470,14 +10463,14 @@
         <v>302</v>
       </c>
       <c r="G100" s="22"/>
-      <c r="J100" s="32" t="s">
+      <c r="I100" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K100" s="22" t="s">
+      <c r="J100" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <v>1805</v>
       </c>
@@ -10491,14 +10484,14 @@
         <v>302</v>
       </c>
       <c r="G101" s="22"/>
-      <c r="J101" s="32" t="s">
+      <c r="I101" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K101" s="22" t="s">
+      <c r="J101" s="22" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="14">
         <v>1806</v>
       </c>
@@ -10512,14 +10505,14 @@
         <v>9</v>
       </c>
       <c r="G102" s="22"/>
-      <c r="J102" s="32" t="s">
+      <c r="I102" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K102" s="22" t="s">
+      <c r="J102" s="22" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <v>1807</v>
       </c>
@@ -10533,14 +10526,14 @@
         <v>4</v>
       </c>
       <c r="G103" s="22"/>
-      <c r="J103" s="32" t="s">
+      <c r="I103" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K103" s="22" t="s">
+      <c r="J103" s="22" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="14">
         <v>1808</v>
       </c>
@@ -10554,14 +10547,14 @@
         <v>302</v>
       </c>
       <c r="G104" s="22"/>
-      <c r="J104" s="32" t="s">
+      <c r="I104" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K104" s="22" t="s">
+      <c r="J104" s="22" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="15">
         <v>1809</v>
       </c>
@@ -10575,14 +10568,14 @@
         <v>302</v>
       </c>
       <c r="G105" s="22"/>
-      <c r="J105" s="32" t="s">
+      <c r="I105" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K105" s="22" t="s">
+      <c r="J105" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="14">
         <v>1810</v>
       </c>
@@ -10596,14 +10589,14 @@
         <v>302</v>
       </c>
       <c r="G106" s="22"/>
-      <c r="J106" s="32" t="s">
+      <c r="I106" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K106" s="22" t="s">
+      <c r="J106" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="15">
         <v>1811</v>
       </c>
@@ -10617,14 +10610,14 @@
         <v>13</v>
       </c>
       <c r="G107" s="22"/>
-      <c r="J107" s="32" t="s">
+      <c r="I107" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K107" s="22" t="s">
+      <c r="J107" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="14">
         <v>1812</v>
       </c>
@@ -10638,14 +10631,14 @@
         <v>13</v>
       </c>
       <c r="G108" s="22"/>
-      <c r="J108" s="32" t="s">
+      <c r="I108" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K108" s="22" t="s">
+      <c r="J108" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="15">
         <v>1813</v>
       </c>
@@ -10659,14 +10652,14 @@
         <v>9</v>
       </c>
       <c r="G109" s="22"/>
-      <c r="J109" s="32" t="s">
+      <c r="I109" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K109" s="22" t="s">
+      <c r="J109" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="14">
         <v>1814</v>
       </c>
@@ -10680,14 +10673,14 @@
         <v>302</v>
       </c>
       <c r="G110" s="22"/>
-      <c r="J110" s="32" t="s">
+      <c r="I110" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K110" s="22" t="s">
+      <c r="J110" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="15">
         <v>1815</v>
       </c>
@@ -10701,14 +10694,14 @@
         <v>13</v>
       </c>
       <c r="G111" s="22"/>
-      <c r="J111" s="32" t="s">
+      <c r="I111" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K111" s="22" t="s">
+      <c r="J111" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="14">
         <v>1816</v>
       </c>
@@ -10722,14 +10715,14 @@
         <v>302</v>
       </c>
       <c r="G112" s="22"/>
-      <c r="J112" s="32" t="s">
+      <c r="I112" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K112" s="22" t="s">
+      <c r="J112" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="15">
         <v>1817</v>
       </c>
@@ -10743,14 +10736,14 @@
         <v>9</v>
       </c>
       <c r="G113" s="22"/>
-      <c r="J113" s="32" t="s">
+      <c r="I113" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K113" s="22" t="s">
+      <c r="J113" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="14">
         <v>1818</v>
       </c>
@@ -10764,14 +10757,14 @@
         <v>13</v>
       </c>
       <c r="G114" s="22"/>
-      <c r="J114" s="32" t="s">
+      <c r="I114" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K114" s="22" t="s">
+      <c r="J114" s="22" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="15">
         <v>1819</v>
       </c>
@@ -10785,14 +10778,14 @@
         <v>13</v>
       </c>
       <c r="G115" s="22"/>
-      <c r="J115" s="32" t="s">
+      <c r="I115" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K115" s="22" t="s">
+      <c r="J115" s="22" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="14">
         <v>1820</v>
       </c>
@@ -10806,14 +10799,14 @@
         <v>9</v>
       </c>
       <c r="G116" s="22"/>
-      <c r="J116" s="32" t="s">
+      <c r="I116" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K116" s="22" t="s">
+      <c r="J116" s="22" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="15">
         <v>1821</v>
       </c>
@@ -10827,14 +10820,14 @@
         <v>302</v>
       </c>
       <c r="G117" s="22"/>
-      <c r="J117" s="32" t="s">
+      <c r="I117" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K117" s="22" t="s">
+      <c r="J117" s="22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="14">
         <v>1822</v>
       </c>
@@ -10848,14 +10841,14 @@
         <v>302</v>
       </c>
       <c r="G118" s="22"/>
-      <c r="J118" s="32" t="s">
+      <c r="I118" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K118" s="22" t="s">
+      <c r="J118" s="22" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="15">
         <v>1823</v>
       </c>
@@ -10869,14 +10862,14 @@
         <v>9</v>
       </c>
       <c r="G119" s="22"/>
-      <c r="J119" s="32" t="s">
+      <c r="I119" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K119" s="22" t="s">
+      <c r="J119" s="22" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="14">
         <v>1824</v>
       </c>
@@ -10890,14 +10883,14 @@
         <v>302</v>
       </c>
       <c r="G120" s="22"/>
-      <c r="J120" s="32" t="s">
+      <c r="I120" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K120" s="22" t="s">
+      <c r="J120" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="15">
         <v>1825</v>
       </c>
@@ -10911,14 +10904,14 @@
         <v>9</v>
       </c>
       <c r="G121" s="22"/>
-      <c r="J121" s="32" t="s">
+      <c r="I121" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K121" s="22" t="s">
+      <c r="J121" s="22" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="14">
         <v>1826</v>
       </c>
@@ -10932,14 +10925,14 @@
         <v>302</v>
       </c>
       <c r="G122" s="22"/>
-      <c r="J122" s="32" t="s">
+      <c r="I122" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K122" s="22" t="s">
+      <c r="J122" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="15">
         <v>1827</v>
       </c>
@@ -10953,14 +10946,14 @@
         <v>9</v>
       </c>
       <c r="G123" s="22"/>
-      <c r="J123" s="32" t="s">
+      <c r="I123" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K123" s="22" t="s">
+      <c r="J123" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="14">
         <v>1828</v>
       </c>
@@ -10974,14 +10967,14 @@
         <v>302</v>
       </c>
       <c r="G124" s="22"/>
-      <c r="J124" s="32" t="s">
+      <c r="I124" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K124" s="22" t="s">
+      <c r="J124" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="15">
         <v>1829</v>
       </c>
@@ -10995,14 +10988,14 @@
         <v>302</v>
       </c>
       <c r="G125" s="22"/>
-      <c r="J125" s="32" t="s">
+      <c r="I125" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K125" s="22" t="s">
+      <c r="J125" s="22" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="14">
         <v>1830</v>
       </c>
@@ -11016,14 +11009,14 @@
         <v>4</v>
       </c>
       <c r="G126" s="22"/>
-      <c r="J126" s="32" t="s">
+      <c r="I126" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K126" s="22" t="s">
+      <c r="J126" s="22" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="15">
         <v>1831</v>
       </c>
@@ -11037,14 +11030,14 @@
         <v>302</v>
       </c>
       <c r="G127" s="22"/>
-      <c r="J127" s="32" t="s">
+      <c r="I127" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K127" s="22" t="s">
+      <c r="J127" s="22" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="14">
         <v>1832</v>
       </c>
@@ -11058,14 +11051,14 @@
         <v>302</v>
       </c>
       <c r="G128" s="22"/>
-      <c r="J128" s="32" t="s">
+      <c r="I128" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K128" s="22" t="s">
+      <c r="J128" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <v>1833</v>
       </c>
@@ -11079,14 +11072,14 @@
         <v>13</v>
       </c>
       <c r="G129" s="22"/>
-      <c r="J129" s="32" t="s">
+      <c r="I129" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K129" s="22" t="s">
+      <c r="J129" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="14">
         <v>1834</v>
       </c>
@@ -11100,14 +11093,14 @@
         <v>9</v>
       </c>
       <c r="G130" s="22"/>
-      <c r="J130" s="32" t="s">
+      <c r="I130" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K130" s="22" t="s">
+      <c r="J130" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="15">
         <v>1835</v>
       </c>
@@ -11121,14 +11114,14 @@
         <v>4</v>
       </c>
       <c r="G131" s="22"/>
-      <c r="J131" s="32" t="s">
+      <c r="I131" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K131" s="22" t="s">
+      <c r="J131" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="14">
         <v>1836</v>
       </c>
@@ -11142,14 +11135,14 @@
         <v>302</v>
       </c>
       <c r="G132" s="22"/>
-      <c r="J132" s="32" t="s">
+      <c r="I132" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K132" s="22" t="s">
+      <c r="J132" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="15">
         <v>1837</v>
       </c>
@@ -11163,14 +11156,14 @@
         <v>302</v>
       </c>
       <c r="G133" s="22"/>
-      <c r="J133" s="32" t="s">
+      <c r="I133" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K133" s="22" t="s">
+      <c r="J133" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="14">
         <v>1838</v>
       </c>
@@ -11184,14 +11177,14 @@
         <v>4</v>
       </c>
       <c r="G134" s="22"/>
-      <c r="J134" s="32" t="s">
+      <c r="I134" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K134" s="22" t="s">
+      <c r="J134" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="15">
         <v>1839</v>
       </c>
@@ -11205,14 +11198,14 @@
         <v>302</v>
       </c>
       <c r="G135" s="22"/>
-      <c r="J135" s="32" t="s">
+      <c r="I135" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K135" s="22" t="s">
+      <c r="J135" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="14">
         <v>1840</v>
       </c>
@@ -11226,14 +11219,14 @@
         <v>302</v>
       </c>
       <c r="G136" s="22"/>
-      <c r="J136" s="32" t="s">
+      <c r="I136" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K136" s="22" t="s">
+      <c r="J136" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="15">
         <v>1841</v>
       </c>
@@ -11247,14 +11240,14 @@
         <v>302</v>
       </c>
       <c r="G137" s="22"/>
-      <c r="J137" s="32" t="s">
+      <c r="I137" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K137" s="22" t="s">
+      <c r="J137" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="14">
         <v>1842</v>
       </c>
@@ -11268,14 +11261,14 @@
         <v>9</v>
       </c>
       <c r="G138" s="22"/>
-      <c r="J138" s="32" t="s">
+      <c r="I138" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K138" s="22" t="s">
+      <c r="J138" s="22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="15">
         <v>1843</v>
       </c>
@@ -11289,14 +11282,14 @@
         <v>4</v>
       </c>
       <c r="G139" s="22"/>
-      <c r="J139" s="32" t="s">
+      <c r="I139" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K139" s="22" t="s">
+      <c r="J139" s="22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="14">
         <v>1844</v>
       </c>
@@ -11310,14 +11303,14 @@
         <v>302</v>
       </c>
       <c r="G140" s="22"/>
-      <c r="J140" s="32" t="s">
+      <c r="I140" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K140" s="22" t="s">
+      <c r="J140" s="22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="15">
         <v>1845</v>
       </c>
@@ -11331,14 +11324,14 @@
         <v>302</v>
       </c>
       <c r="G141" s="22"/>
-      <c r="J141" s="32" t="s">
+      <c r="I141" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K141" s="22" t="s">
+      <c r="J141" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="14">
         <v>1846</v>
       </c>
@@ -11352,14 +11345,14 @@
         <v>9</v>
       </c>
       <c r="G142" s="22"/>
-      <c r="J142" s="32" t="s">
+      <c r="I142" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K142" s="22" t="s">
+      <c r="J142" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="15">
         <v>1847</v>
       </c>
@@ -11373,14 +11366,14 @@
         <v>13</v>
       </c>
       <c r="G143" s="22"/>
-      <c r="J143" s="32" t="s">
+      <c r="I143" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K143" s="22" t="s">
+      <c r="J143" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="14">
         <v>1848</v>
       </c>
@@ -11394,14 +11387,14 @@
         <v>13</v>
       </c>
       <c r="G144" s="22"/>
-      <c r="J144" s="32" t="s">
+      <c r="I144" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K144" s="22" t="s">
+      <c r="J144" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="15">
         <v>1849</v>
       </c>
@@ -11415,14 +11408,14 @@
         <v>9</v>
       </c>
       <c r="G145" s="22"/>
-      <c r="J145" s="32" t="s">
+      <c r="I145" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K145" s="22" t="s">
+      <c r="J145" s="22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="14">
         <v>1850</v>
       </c>
@@ -11436,14 +11429,14 @@
         <v>302</v>
       </c>
       <c r="G146" s="22"/>
-      <c r="J146" s="32" t="s">
+      <c r="I146" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K146" s="22" t="s">
+      <c r="J146" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="15">
         <v>1851</v>
       </c>
@@ -11457,14 +11450,14 @@
         <v>13</v>
       </c>
       <c r="G147" s="22"/>
-      <c r="J147" s="32" t="s">
+      <c r="I147" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K147" s="22" t="s">
+      <c r="J147" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="14">
         <v>1852</v>
       </c>
@@ -11478,14 +11471,14 @@
         <v>9</v>
       </c>
       <c r="G148" s="22"/>
-      <c r="J148" s="32" t="s">
+      <c r="I148" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K148" s="22" t="s">
+      <c r="J148" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="15">
         <v>1853</v>
       </c>
@@ -11499,14 +11492,14 @@
         <v>4</v>
       </c>
       <c r="G149" s="22"/>
-      <c r="J149" s="32" t="s">
+      <c r="I149" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K149" s="22" t="s">
+      <c r="J149" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="14">
         <v>1854</v>
       </c>
@@ -11520,14 +11513,14 @@
         <v>13</v>
       </c>
       <c r="G150" s="22"/>
-      <c r="J150" s="32" t="s">
+      <c r="I150" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K150" s="22" t="s">
+      <c r="J150" s="22" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <v>1855</v>
       </c>
@@ -11541,14 +11534,14 @@
         <v>13</v>
       </c>
       <c r="G151" s="22"/>
-      <c r="J151" s="32" t="s">
+      <c r="I151" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K151" s="22" t="s">
+      <c r="J151" s="22" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="14">
         <v>1856</v>
       </c>
@@ -11562,14 +11555,14 @@
         <v>302</v>
       </c>
       <c r="G152" s="22"/>
-      <c r="J152" s="32" t="s">
+      <c r="I152" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K152" s="22" t="s">
+      <c r="J152" s="22" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="15">
         <v>1857</v>
       </c>
@@ -11583,14 +11576,14 @@
         <v>302</v>
       </c>
       <c r="G153" s="22"/>
-      <c r="J153" s="32" t="s">
+      <c r="I153" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K153" s="22" t="s">
+      <c r="J153" s="22" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="14">
         <v>1858</v>
       </c>
@@ -11604,14 +11597,14 @@
         <v>9</v>
       </c>
       <c r="G154" s="22"/>
-      <c r="J154" s="32" t="s">
+      <c r="I154" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K154" s="22" t="s">
+      <c r="J154" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="15">
         <v>1859</v>
       </c>
@@ -11625,14 +11618,14 @@
         <v>302</v>
       </c>
       <c r="G155" s="22"/>
-      <c r="J155" s="32" t="s">
+      <c r="I155" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K155" s="22" t="s">
+      <c r="J155" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="14">
         <v>1860</v>
       </c>
@@ -11646,14 +11639,14 @@
         <v>9</v>
       </c>
       <c r="G156" s="22"/>
-      <c r="J156" s="32" t="s">
+      <c r="I156" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K156" s="22" t="s">
+      <c r="J156" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="15">
         <v>1861</v>
       </c>
@@ -11667,14 +11660,14 @@
         <v>302</v>
       </c>
       <c r="G157" s="22"/>
-      <c r="J157" s="32" t="s">
+      <c r="I157" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K157" s="22" t="s">
+      <c r="J157" s="22" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="14">
         <v>1862</v>
       </c>
@@ -11688,14 +11681,14 @@
         <v>302</v>
       </c>
       <c r="G158" s="22"/>
-      <c r="J158" s="32" t="s">
+      <c r="I158" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K158" s="22" t="s">
+      <c r="J158" s="22" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="15">
         <v>1863</v>
       </c>
@@ -11709,14 +11702,14 @@
         <v>9</v>
       </c>
       <c r="G159" s="22"/>
-      <c r="J159" s="32" t="s">
+      <c r="I159" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K159" s="22" t="s">
+      <c r="J159" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="14">
         <v>1864</v>
       </c>
@@ -11730,14 +11723,14 @@
         <v>302</v>
       </c>
       <c r="G160" s="22"/>
-      <c r="J160" s="32" t="s">
+      <c r="I160" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K160" s="22" t="s">
+      <c r="J160" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="15">
         <v>1865</v>
       </c>
@@ -11751,14 +11744,14 @@
         <v>302</v>
       </c>
       <c r="G161" s="22"/>
-      <c r="J161" s="32" t="s">
+      <c r="I161" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K161" s="22" t="s">
+      <c r="J161" s="22" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="14">
         <v>1866</v>
       </c>
@@ -11772,14 +11765,14 @@
         <v>9</v>
       </c>
       <c r="G162" s="22"/>
-      <c r="J162" s="32" t="s">
+      <c r="I162" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K162" s="22" t="s">
+      <c r="J162" s="22" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="15">
         <v>1867</v>
       </c>
@@ -11793,14 +11786,14 @@
         <v>302</v>
       </c>
       <c r="G163" s="22"/>
-      <c r="J163" s="32" t="s">
+      <c r="I163" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K163" s="22" t="s">
+      <c r="J163" s="22" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="14">
         <v>1868</v>
       </c>
@@ -11814,14 +11807,14 @@
         <v>302</v>
       </c>
       <c r="G164" s="22"/>
-      <c r="J164" s="32" t="s">
+      <c r="I164" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K164" s="22" t="s">
+      <c r="J164" s="22" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="15">
         <v>1869</v>
       </c>
@@ -11835,14 +11828,14 @@
         <v>13</v>
       </c>
       <c r="G165" s="22"/>
-      <c r="J165" s="32" t="s">
+      <c r="I165" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K165" s="22" t="s">
+      <c r="J165" s="22" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="14">
         <v>1870</v>
       </c>
@@ -11856,14 +11849,14 @@
         <v>4</v>
       </c>
       <c r="G166" s="22"/>
-      <c r="J166" s="32" t="s">
+      <c r="I166" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K166" s="22" t="s">
+      <c r="J166" s="22" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="15">
         <v>1871</v>
       </c>
@@ -11877,14 +11870,14 @@
         <v>4</v>
       </c>
       <c r="G167" s="22"/>
-      <c r="J167" s="32" t="s">
+      <c r="I167" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K167" s="22" t="s">
+      <c r="J167" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="14">
         <v>1872</v>
       </c>
@@ -11898,14 +11891,14 @@
         <v>302</v>
       </c>
       <c r="G168" s="22"/>
-      <c r="J168" s="32" t="s">
+      <c r="I168" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K168" s="22" t="s">
+      <c r="J168" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="15">
         <v>1873</v>
       </c>
@@ -11919,14 +11912,14 @@
         <v>302</v>
       </c>
       <c r="G169" s="22"/>
-      <c r="J169" s="32" t="s">
+      <c r="I169" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K169" s="22" t="s">
+      <c r="J169" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="14">
         <v>1874</v>
       </c>
@@ -11940,14 +11933,14 @@
         <v>4</v>
       </c>
       <c r="G170" s="22"/>
-      <c r="J170" s="32" t="s">
+      <c r="I170" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K170" s="22" t="s">
+      <c r="J170" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="15">
         <v>1875</v>
       </c>
@@ -11961,14 +11954,14 @@
         <v>302</v>
       </c>
       <c r="G171" s="22"/>
-      <c r="J171" s="32" t="s">
+      <c r="I171" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K171" s="22" t="s">
+      <c r="J171" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="14">
         <v>1876</v>
       </c>
@@ -11982,14 +11975,14 @@
         <v>302</v>
       </c>
       <c r="G172" s="22"/>
-      <c r="J172" s="32" t="s">
+      <c r="I172" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K172" s="22" t="s">
+      <c r="J172" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="15">
         <v>1877</v>
       </c>
@@ -12003,14 +11996,14 @@
         <v>302</v>
       </c>
       <c r="G173" s="22"/>
-      <c r="J173" s="32" t="s">
+      <c r="I173" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K173" s="22" t="s">
+      <c r="J173" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="14">
         <v>1878</v>
       </c>
@@ -12024,14 +12017,14 @@
         <v>9</v>
       </c>
       <c r="G174" s="22"/>
-      <c r="J174" s="32" t="s">
+      <c r="I174" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K174" s="22" t="s">
+      <c r="J174" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="15">
         <v>1879</v>
       </c>
@@ -12045,14 +12038,14 @@
         <v>9</v>
       </c>
       <c r="G175" s="22"/>
-      <c r="J175" s="32" t="s">
+      <c r="I175" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K175" s="22" t="s">
+      <c r="J175" s="22" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="14">
         <v>1880</v>
       </c>
@@ -12066,14 +12059,14 @@
         <v>302</v>
       </c>
       <c r="G176" s="22"/>
-      <c r="J176" s="32" t="s">
+      <c r="I176" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K176" s="22" t="s">
+      <c r="J176" s="22" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="15">
         <v>1881</v>
       </c>
@@ -12087,14 +12080,14 @@
         <v>302</v>
       </c>
       <c r="G177" s="22"/>
-      <c r="J177" s="32" t="s">
+      <c r="I177" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K177" s="22" t="s">
+      <c r="J177" s="22" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="14">
         <v>1882</v>
       </c>
@@ -12108,14 +12101,14 @@
         <v>302</v>
       </c>
       <c r="G178" s="22"/>
-      <c r="J178" s="32" t="s">
+      <c r="I178" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K178" s="22" t="s">
+      <c r="J178" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="15">
         <v>1883</v>
       </c>
@@ -12129,14 +12122,14 @@
         <v>13</v>
       </c>
       <c r="G179" s="22"/>
-      <c r="J179" s="32" t="s">
+      <c r="I179" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K179" s="22" t="s">
+      <c r="J179" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="14">
         <v>1884</v>
       </c>
@@ -12150,14 +12143,14 @@
         <v>13</v>
       </c>
       <c r="G180" s="22"/>
-      <c r="J180" s="32" t="s">
+      <c r="I180" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K180" s="22" t="s">
+      <c r="J180" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="15">
         <v>1885</v>
       </c>
@@ -12171,14 +12164,14 @@
         <v>9</v>
       </c>
       <c r="G181" s="22"/>
-      <c r="J181" s="32" t="s">
+      <c r="I181" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K181" s="22" t="s">
+      <c r="J181" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="14">
         <v>1886</v>
       </c>
@@ -12192,14 +12185,14 @@
         <v>9</v>
       </c>
       <c r="G182" s="22"/>
-      <c r="J182" s="32" t="s">
+      <c r="I182" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K182" s="22" t="s">
+      <c r="J182" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="15">
         <v>1887</v>
       </c>
@@ -12213,14 +12206,14 @@
         <v>13</v>
       </c>
       <c r="G183" s="22"/>
-      <c r="J183" s="32" t="s">
+      <c r="I183" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K183" s="22" t="s">
+      <c r="J183" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="14">
         <v>1888</v>
       </c>
@@ -12234,14 +12227,14 @@
         <v>302</v>
       </c>
       <c r="G184" s="22"/>
-      <c r="J184" s="32" t="s">
+      <c r="I184" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K184" s="22" t="s">
+      <c r="J184" s="22" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="15">
         <v>1889</v>
       </c>
@@ -12255,14 +12248,14 @@
         <v>4</v>
       </c>
       <c r="G185" s="22"/>
-      <c r="J185" s="32" t="s">
+      <c r="I185" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K185" s="22" t="s">
+      <c r="J185" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="14">
         <v>1890</v>
       </c>
@@ -12276,14 +12269,14 @@
         <v>13</v>
       </c>
       <c r="G186" s="22"/>
-      <c r="J186" s="32" t="s">
+      <c r="I186" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K186" s="22" t="s">
+      <c r="J186" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="15">
         <v>1891</v>
       </c>
@@ -12297,14 +12290,14 @@
         <v>13</v>
       </c>
       <c r="G187" s="22"/>
-      <c r="J187" s="32" t="s">
+      <c r="I187" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K187" s="22" t="s">
+      <c r="J187" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="14">
         <v>1892</v>
       </c>
@@ -12318,14 +12311,14 @@
         <v>302</v>
       </c>
       <c r="G188" s="22"/>
-      <c r="J188" s="32" t="s">
+      <c r="I188" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K188" s="22" t="s">
+      <c r="J188" s="22" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="15">
         <v>1893</v>
       </c>
@@ -12339,14 +12332,14 @@
         <v>302</v>
       </c>
       <c r="G189" s="22"/>
-      <c r="J189" s="32" t="s">
+      <c r="I189" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K189" s="22" t="s">
+      <c r="J189" s="22" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="14">
         <v>1894</v>
       </c>
@@ -12360,14 +12353,14 @@
         <v>9</v>
       </c>
       <c r="G190" s="22"/>
-      <c r="J190" s="32" t="s">
+      <c r="I190" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K190" s="22" t="s">
+      <c r="J190" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="15">
         <v>1895</v>
       </c>
@@ -12381,14 +12374,14 @@
         <v>302</v>
       </c>
       <c r="G191" s="22"/>
-      <c r="J191" s="32" t="s">
+      <c r="I191" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K191" s="22" t="s">
+      <c r="J191" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="14">
         <v>1896</v>
       </c>
@@ -12402,14 +12395,14 @@
         <v>9</v>
       </c>
       <c r="G192" s="22"/>
-      <c r="J192" s="32" t="s">
+      <c r="I192" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K192" s="22" t="s">
+      <c r="J192" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="15">
         <v>1897</v>
       </c>
@@ -12423,14 +12416,14 @@
         <v>302</v>
       </c>
       <c r="G193" s="22"/>
-      <c r="J193" s="32" t="s">
+      <c r="I193" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K193" s="22" t="s">
+      <c r="J193" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="14">
         <v>1898</v>
       </c>
@@ -12444,14 +12437,14 @@
         <v>302</v>
       </c>
       <c r="G194" s="22"/>
-      <c r="J194" s="32" t="s">
+      <c r="I194" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K194" s="22" t="s">
+      <c r="J194" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="15">
         <v>1899</v>
       </c>
@@ -12465,14 +12458,14 @@
         <v>302</v>
       </c>
       <c r="G195" s="22"/>
-      <c r="J195" s="32" t="s">
+      <c r="I195" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K195" s="22" t="s">
+      <c r="J195" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="14">
         <v>1900</v>
       </c>
@@ -12486,14 +12479,14 @@
         <v>9</v>
       </c>
       <c r="G196" s="22"/>
-      <c r="J196" s="32" t="s">
+      <c r="I196" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K196" s="22" t="s">
+      <c r="J196" s="22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="15">
         <v>1901</v>
       </c>
@@ -12507,14 +12500,14 @@
         <v>302</v>
       </c>
       <c r="G197" s="22"/>
-      <c r="J197" s="32" t="s">
+      <c r="I197" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K197" s="22" t="s">
+      <c r="J197" s="22" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="14">
         <v>1902</v>
       </c>
@@ -12528,14 +12521,14 @@
         <v>4</v>
       </c>
       <c r="G198" s="22"/>
-      <c r="J198" s="32" t="s">
+      <c r="I198" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K198" s="22" t="s">
+      <c r="J198" s="22" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="15">
         <v>1903</v>
       </c>
@@ -12549,14 +12542,14 @@
         <v>302</v>
       </c>
       <c r="G199" s="22"/>
-      <c r="J199" s="32" t="s">
+      <c r="I199" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K199" s="22" t="s">
+      <c r="J199" s="22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="14">
         <v>1904</v>
       </c>
@@ -12570,14 +12563,14 @@
         <v>302</v>
       </c>
       <c r="G200" s="22"/>
-      <c r="J200" s="32" t="s">
+      <c r="I200" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K200" s="22" t="s">
+      <c r="J200" s="22" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="15">
         <v>1905</v>
       </c>
@@ -12591,14 +12584,14 @@
         <v>13</v>
       </c>
       <c r="G201" s="22"/>
-      <c r="J201" s="32" t="s">
+      <c r="I201" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K201" s="22" t="s">
+      <c r="J201" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="14">
         <v>1906</v>
       </c>
@@ -12612,14 +12605,14 @@
         <v>4</v>
       </c>
       <c r="G202" s="22"/>
-      <c r="J202" s="32" t="s">
+      <c r="I202" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K202" s="22" t="s">
+      <c r="J202" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="15">
         <v>1907</v>
       </c>
@@ -12633,14 +12626,14 @@
         <v>4</v>
       </c>
       <c r="G203" s="22"/>
-      <c r="J203" s="32" t="s">
+      <c r="I203" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K203" s="22" t="s">
+      <c r="J203" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="14">
         <v>1908</v>
       </c>
@@ -12654,14 +12647,14 @@
         <v>302</v>
       </c>
       <c r="G204" s="22"/>
-      <c r="J204" s="32" t="s">
+      <c r="I204" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K204" s="22" t="s">
+      <c r="J204" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="15">
         <v>1909</v>
       </c>
@@ -12675,14 +12668,14 @@
         <v>9</v>
       </c>
       <c r="G205" s="22"/>
-      <c r="J205" s="32" t="s">
+      <c r="I205" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K205" s="22" t="s">
+      <c r="J205" s="22" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="14">
         <v>1910</v>
       </c>
@@ -12696,14 +12689,14 @@
         <v>4</v>
       </c>
       <c r="G206" s="22"/>
-      <c r="J206" s="32" t="s">
+      <c r="I206" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K206" s="22" t="s">
+      <c r="J206" s="22" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="15">
         <v>1911</v>
       </c>
@@ -12717,14 +12710,14 @@
         <v>302</v>
       </c>
       <c r="G207" s="22"/>
-      <c r="J207" s="32" t="s">
+      <c r="I207" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K207" s="22" t="s">
+      <c r="J207" s="22" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="14">
         <v>1912</v>
       </c>
@@ -12738,14 +12731,14 @@
         <v>302</v>
       </c>
       <c r="G208" s="22"/>
-      <c r="J208" s="32" t="s">
+      <c r="I208" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K208" s="22" t="s">
+      <c r="J208" s="22" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="15">
         <v>1913</v>
       </c>
@@ -12759,14 +12752,14 @@
         <v>302</v>
       </c>
       <c r="G209" s="22"/>
-      <c r="J209" s="32" t="s">
+      <c r="I209" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K209" s="22" t="s">
+      <c r="J209" s="22" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="14">
         <v>1914</v>
       </c>
@@ -12780,14 +12773,14 @@
         <v>9</v>
       </c>
       <c r="G210" s="22"/>
-      <c r="J210" s="32" t="s">
+      <c r="I210" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="K210" s="22" t="s">
+      <c r="J210" s="22" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="15">
         <v>1915</v>
       </c>
@@ -12801,14 +12794,14 @@
         <v>4</v>
       </c>
       <c r="G211" s="22"/>
-      <c r="J211" s="32" t="s">
+      <c r="I211" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="K211" s="22" t="s">
+      <c r="J211" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="14">
         <v>1916</v>
       </c>
@@ -12822,14 +12815,14 @@
         <v>302</v>
       </c>
       <c r="G212" s="22"/>
-      <c r="J212" s="32" t="s">
+      <c r="I212" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K212" s="22" t="s">
+      <c r="J212" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="15">
         <v>1917</v>
       </c>
@@ -12843,14 +12836,14 @@
         <v>302</v>
       </c>
       <c r="G213" s="22"/>
-      <c r="J213" s="32" t="s">
+      <c r="I213" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K213" s="22" t="s">
+      <c r="J213" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="14">
         <v>1918</v>
       </c>
@@ -12864,14 +12857,14 @@
         <v>302</v>
       </c>
       <c r="G214" s="22"/>
-      <c r="J214" s="32" t="s">
+      <c r="I214" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K214" s="22" t="s">
+      <c r="J214" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="15">
         <v>1919</v>
       </c>
@@ -12885,14 +12878,14 @@
         <v>13</v>
       </c>
       <c r="G215" s="22"/>
-      <c r="J215" s="32" t="s">
+      <c r="I215" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K215" s="22" t="s">
+      <c r="J215" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="14">
         <v>1920</v>
       </c>
@@ -12906,14 +12899,14 @@
         <v>13</v>
       </c>
       <c r="G216" s="22"/>
-      <c r="J216" s="32" t="s">
+      <c r="I216" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K216" s="22" t="s">
+      <c r="J216" s="22" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="15">
         <v>1921</v>
       </c>
@@ -12927,84 +12920,84 @@
         <v>9</v>
       </c>
       <c r="G217" s="22"/>
-      <c r="J217" s="32" t="s">
+      <c r="I217" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K217" s="22" t="s">
+      <c r="J217" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K218" s="22"/>
-    </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K219" s="22"/>
-    </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K220" s="22"/>
-    </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K221" s="22"/>
-    </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K222" s="22"/>
-    </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K223" s="22"/>
-    </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K224" s="22"/>
-    </row>
-    <row r="225" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K225" s="22"/>
-    </row>
-    <row r="226" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K226" s="22"/>
-    </row>
-    <row r="227" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K227" s="22"/>
-    </row>
-    <row r="228" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K228" s="22"/>
-    </row>
-    <row r="229" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K229" s="22"/>
-    </row>
-    <row r="230" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K230" s="22"/>
-    </row>
-    <row r="231" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K231" s="22"/>
-    </row>
-    <row r="232" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K232" s="22"/>
-    </row>
-    <row r="233" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K233" s="22"/>
-    </row>
-    <row r="234" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K234" s="22"/>
-    </row>
-    <row r="235" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K235" s="22"/>
-    </row>
-    <row r="236" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K236" s="22"/>
-    </row>
-    <row r="237" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K237" s="22"/>
-    </row>
-    <row r="238" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K238" s="22"/>
-    </row>
-    <row r="239" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K239" s="22"/>
-    </row>
-    <row r="240" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K240" s="22"/>
-    </row>
-    <row r="241" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K241" s="22"/>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J218" s="22"/>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J219" s="22"/>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J220" s="22"/>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J221" s="22"/>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J222" s="22"/>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J223" s="22"/>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J224" s="22"/>
+    </row>
+    <row r="225" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J225" s="22"/>
+    </row>
+    <row r="226" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J226" s="22"/>
+    </row>
+    <row r="227" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J227" s="22"/>
+    </row>
+    <row r="228" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J228" s="22"/>
+    </row>
+    <row r="229" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J229" s="22"/>
+    </row>
+    <row r="230" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J230" s="22"/>
+    </row>
+    <row r="231" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J231" s="22"/>
+    </row>
+    <row r="232" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J232" s="22"/>
+    </row>
+    <row r="233" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J233" s="22"/>
+    </row>
+    <row r="234" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J234" s="22"/>
+    </row>
+    <row r="235" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J235" s="22"/>
+    </row>
+    <row r="236" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J236" s="22"/>
+    </row>
+    <row r="237" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J237" s="22"/>
+    </row>
+    <row r="238" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J238" s="22"/>
+    </row>
+    <row r="239" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J239" s="22"/>
+    </row>
+    <row r="240" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J240" s="22"/>
+    </row>
+    <row r="241" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J241" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -13019,7 +13012,7 @@
   <dimension ref="A1:H336"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E231" sqref="E231"/>
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19071,8 +19064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I746"/>
   <sheetViews>
-    <sheetView topLeftCell="A711" workbookViewId="0">
-      <selection activeCell="A728" sqref="A728:XFD728"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30177,7 +30170,7 @@
   <dimension ref="B1:D51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30629,8 +30622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1136" workbookViewId="0">
-      <selection activeCell="H1168" sqref="H1168"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62803,7 +62796,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62990,7 +62983,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D19" sqref="A1:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63015,10 +63008,10 @@
         <v>12</v>
       </c>
       <c r="D1" s="32" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>1518</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>1519</v>
       </c>
       <c r="F1" s="32" t="s">
         <v>7</v>
@@ -63032,21 +63025,24 @@
         <v>1</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>15</v>
+        <v>313</v>
       </c>
       <c r="E2" s="32">
         <v>0</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" s="32">
         <v>1</v>
       </c>
+      <c r="D3" s="32" t="s">
+        <v>15</v>
+      </c>
       <c r="F3" s="32" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -63054,7 +63050,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -63062,23 +63058,29 @@
         <v>1</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" s="32">
         <v>1</v>
       </c>
+      <c r="D6" s="32" t="s">
+        <v>312</v>
+      </c>
       <c r="F6" s="32" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" s="32">
         <v>0</v>
       </c>
+      <c r="D7" s="32" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="32" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -63086,7 +63088,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -63094,7 +63096,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -63104,32 +63106,44 @@
       <c r="C10" s="32">
         <v>1</v>
       </c>
+      <c r="D10" s="32" t="s">
+        <v>320</v>
+      </c>
       <c r="F10" s="32" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" s="32">
         <v>1</v>
       </c>
+      <c r="D11" s="32" t="s">
+        <v>15</v>
+      </c>
       <c r="F11" s="32" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" s="32">
         <v>0</v>
       </c>
+      <c r="D12" s="32" t="s">
+        <v>321</v>
+      </c>
       <c r="F12" s="32" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="32">
         <v>0</v>
       </c>
+      <c r="D13" s="32" t="s">
+        <v>15</v>
+      </c>
       <c r="F13" s="32" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -63137,7 +63151,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -63145,7 +63159,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -63153,7 +63167,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -63163,16 +63177,22 @@
       <c r="C17" s="32">
         <v>1</v>
       </c>
+      <c r="D17" s="32" t="s">
+        <v>316</v>
+      </c>
       <c r="F17" s="32" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C18" s="32">
         <v>1</v>
       </c>
+      <c r="D18" s="32" t="s">
+        <v>15</v>
+      </c>
       <c r="F18" s="32" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -63180,7 +63200,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -63188,7 +63208,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -63196,15 +63216,18 @@
         <v>0</v>
       </c>
       <c r="F21" s="32" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C22" s="32">
         <v>1</v>
       </c>
+      <c r="D22" s="32" t="s">
+        <v>314</v>
+      </c>
       <c r="F22" s="32" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>